<commit_message>
Implemented basic stage shifting code, renamed chargeLimit to charge (current) and introduced chargeMax (max charge) variable instead
</commit_message>
<xml_diff>
--- a/stages.xlsx
+++ b/stages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>playerSpeed</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Player</t>
-  </si>
-  <si>
-    <t>chargeLimit</t>
   </si>
   <si>
     <t>healthDrain</t>
@@ -199,6 +196,12 @@
   </si>
   <si>
     <t>Moving to the right = faster time, moving to left = slower time</t>
+  </si>
+  <si>
+    <t>chargeMax</t>
+  </si>
+  <si>
+    <t>max</t>
   </si>
 </sst>
 </file>
@@ -363,6 +366,41 @@
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -372,41 +410,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -696,307 +699,312 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="10"/>
+    <col min="12" max="12" width="41.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="7"/>
     <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>33</v>
+      <c r="K2" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5">
         <v>4</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="6">
         <v>5000</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="6">
         <v>100</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>10</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="11">
         <v>100</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="6">
         <v>500</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="11">
         <v>4</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <v>100</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>8</v>
+      <c r="L3" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="21">
+        <v>10</v>
+      </c>
+      <c r="I4" s="12">
         <v>150</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>42</v>
+      <c r="L4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
         <v>6</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>50</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="6">
         <v>250</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="8">
         <v>8</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="12">
         <v>175</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>13</v>
+      <c r="L5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>200</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="2">
         <v>20</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="6">
         <v>1000</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="8">
         <v>2</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>75</v>
       </c>
-      <c r="J6" s="9" t="s">
-        <v>24</v>
+      <c r="J6" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="6">
+        <v>37</v>
+      </c>
+      <c r="C8" s="3">
         <v>2500</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="2">
         <v>20</v>
       </c>
       <c r="F8" s="1">
         <v>200</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="12">
         <v>200</v>
       </c>
-      <c r="J8" s="20" t="s">
-        <v>51</v>
+      <c r="J8" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0</v>
-      </c>
-      <c r="F9" s="27" t="s">
+      <c r="J9" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" t="s">
-        <v>50</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K11" s="9"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="8" t="s">
         <v>16</v>
-      </c>
-      <c r="L35" s="11" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated version of stages spreadsheet
</commit_message>
<xml_diff>
--- a/stages.xlsx
+++ b/stages.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominic\Documents\Programming\Projects\Rewind\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10650" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>playerSpeed</t>
   </si>
@@ -56,9 +51,6 @@
     <t>timeDown</t>
   </si>
   <si>
-    <t>upsideDown</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -80,9 +72,6 @@
     <t>modDesc</t>
   </si>
   <si>
-    <t>stage is upside down</t>
-  </si>
-  <si>
     <t>powerDesc</t>
   </si>
   <si>
@@ -98,9 +87,6 @@
     <t>speedUp</t>
   </si>
   <si>
-    <t>stop</t>
-  </si>
-  <si>
     <t>can move while rest of stage is paused</t>
   </si>
   <si>
@@ -110,13 +96,7 @@
     <t>point and click to teleport</t>
   </si>
   <si>
-    <t>randScore</t>
-  </si>
-  <si>
     <t>score multiplier is randomised</t>
-  </si>
-  <si>
-    <t>volatile</t>
   </si>
   <si>
     <t>increases score multiplier volatility - higher max, lower min, less of in between</t>
@@ -189,19 +169,46 @@
     <t>"ghost mode"</t>
   </si>
   <si>
-    <t>vamp</t>
-  </si>
-  <si>
     <t>spaceTime</t>
   </si>
   <si>
     <t>Moving to the right = faster time, moving to left = slower time</t>
   </si>
   <si>
+    <t>Jump higher, projectiles bounce?</t>
+  </si>
+  <si>
+    <t>timeStop</t>
+  </si>
+  <si>
+    <t>hpVamp</t>
+  </si>
+  <si>
+    <t>lowGrav</t>
+  </si>
+  <si>
+    <t>stage is upside down, left/right swapped, projectile absorption behaviour reversed</t>
+  </si>
+  <si>
+    <t>anti</t>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>send out own orbs to cancel out ones on screen + earn points</t>
+  </si>
+  <si>
+    <t>Invert colours</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
     <t>chargeMax</t>
-  </si>
-  <si>
-    <t>max</t>
   </si>
 </sst>
 </file>
@@ -363,12 +370,11 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -382,7 +388,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -409,6 +414,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -688,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -699,152 +719,161 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="72.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="7"/>
+    <col min="12" max="12" width="76.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="6"/>
     <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="22" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="24"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="22"/>
       <c r="O1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="15" t="s">
+      <c r="F2" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="L2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>32</v>
+      <c r="N2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="5">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>5000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>100</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>10</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>100</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>500</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="10">
         <v>4</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>100</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>24</v>
+      <c r="J3" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="12">
+        <v>52</v>
+      </c>
+      <c r="I4" s="11">
         <v>150</v>
       </c>
+      <c r="J4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>41</v>
+        <v>51</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -860,23 +889,23 @@
       <c r="E5" s="2">
         <v>10</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="3">
         <v>250</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <v>8</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>175</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>21</v>
+      <c r="J5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -892,45 +921,66 @@
       <c r="E6" s="2">
         <v>20</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="3">
         <v>1000</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <v>2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="11">
         <v>75</v>
       </c>
-      <c r="J6" s="6" t="s">
-        <v>23</v>
+      <c r="J6" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="K6" t="s">
         <v>22</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>30</v>
+        <v>56</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="K7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3">
         <v>2500</v>
@@ -941,22 +991,22 @@
       <c r="F8" s="1">
         <v>200</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>200</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>50</v>
+      <c r="J8" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -964,47 +1014,51 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>48</v>
+      <c r="F9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="11">
+        <v>250</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>26</v>
+        <v>45</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="K11" s="6"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>54</v>
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="L35" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="L35" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1014,6 +1068,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commented out code for stage "anti" (incomplete), remade stage 1 to be timeUp
</commit_message>
<xml_diff>
--- a/stages.xlsx
+++ b/stages.xlsx
@@ -388,6 +388,21 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -414,21 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -708,7 +708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -719,7 +719,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,25 +742,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="17" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20" t="s">
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="22"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27"/>
       <c r="O1" s="1" t="s">
         <v>29</v>
       </c>
@@ -887,7 +887,7 @@
         <v>50</v>
       </c>
       <c r="E5" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3">
         <v>250</v>
@@ -919,7 +919,7 @@
         <v>200</v>
       </c>
       <c r="E6" s="2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="G6" s="3">
         <v>1000</v>
@@ -944,28 +944,28 @@
       <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="17" t="s">
         <v>31</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -1014,7 +1014,7 @@
       <c r="E9" s="2">
         <v>0</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="18" t="s">
         <v>40</v>
       </c>
       <c r="I9" s="11">

</xml_diff>

<commit_message>
Updated stage spreadsheet, rearranged Stage class to fit order on the spreadsheet
</commit_message>
<xml_diff>
--- a/stages.xlsx
+++ b/stages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>playerSpeed</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>chargeGain</t>
+  </si>
+  <si>
+    <t>healthLoss</t>
   </si>
 </sst>
 </file>
@@ -393,33 +396,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
@@ -435,6 +411,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -721,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,45 +737,47 @@
     <col min="3" max="3" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="71.28515625" customWidth="1"/>
-    <col min="13" max="13" width="76.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="5"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="71.28515625" customWidth="1"/>
+    <col min="14" max="14" width="76.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="5"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="17" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="1" t="s">
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>32</v>
       </c>
@@ -789,40 +794,43 @@
         <v>3</v>
       </c>
       <c r="F2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="L2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -839,315 +847,327 @@
         <v>10</v>
       </c>
       <c r="F3" s="8">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8">
+        <v>400</v>
+      </c>
+      <c r="H3" s="8">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4">
+        <v>500</v>
+      </c>
+      <c r="J3" s="8">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4">
         <v>100</v>
       </c>
-      <c r="G3" s="8">
-        <v>5</v>
-      </c>
-      <c r="H3" s="4">
-        <v>500</v>
-      </c>
-      <c r="I3" s="8">
-        <v>4</v>
-      </c>
-      <c r="J3" s="4">
-        <v>100</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>18</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="3">
-        <v>4</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="10">
+        <v>6</v>
       </c>
       <c r="C4" s="4">
         <v>5000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="11">
+        <v>50</v>
+      </c>
+      <c r="E4" s="10">
+        <v>20</v>
+      </c>
+      <c r="F4" s="11">
+        <v>20</v>
+      </c>
+      <c r="G4" s="11">
+        <v>600</v>
+      </c>
+      <c r="H4" s="11">
+        <v>5</v>
+      </c>
+      <c r="I4" s="11">
+        <v>250</v>
+      </c>
+      <c r="J4" s="11">
+        <v>10</v>
+      </c>
+      <c r="K4" s="9">
+        <v>175</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11">
+        <v>2500</v>
+      </c>
+      <c r="D5" s="4">
         <v>100</v>
-      </c>
-      <c r="E4" s="3">
-        <v>10</v>
-      </c>
-      <c r="F4" s="8">
-        <v>100</v>
-      </c>
-      <c r="G4" s="8">
-        <v>5</v>
-      </c>
-      <c r="H4" s="8">
-        <v>500</v>
-      </c>
-      <c r="I4" s="8">
-        <v>4</v>
-      </c>
-      <c r="J4" s="9">
-        <v>150</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="10">
-        <v>6</v>
-      </c>
-      <c r="C5" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="11">
-        <v>50</v>
       </c>
       <c r="E5" s="10">
         <v>20</v>
       </c>
-      <c r="G5" s="11">
+      <c r="F5" s="11">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9">
+        <v>800</v>
+      </c>
+      <c r="H5" s="20">
+        <v>10</v>
+      </c>
+      <c r="I5">
+        <v>500</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+      <c r="K5" s="9">
+        <v>200</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10">
         <v>2</v>
       </c>
-      <c r="H5" s="11">
+      <c r="C12" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D12" s="11">
+        <v>200</v>
+      </c>
+      <c r="E12" s="10">
+        <v>5</v>
+      </c>
+      <c r="H12" s="11">
+        <v>5</v>
+      </c>
+      <c r="I12" s="11">
+        <v>1000</v>
+      </c>
+      <c r="J12" s="11">
+        <v>2</v>
+      </c>
+      <c r="K12" s="9">
+        <v>75</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5000</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="20">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>500</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14" s="9">
         <v>250</v>
       </c>
-      <c r="I5" s="11">
-        <v>8</v>
-      </c>
-      <c r="J5" s="9">
-        <v>175</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>9</v>
+      <c r="L14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="M14" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="10">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="M16" s="4"/>
+      <c r="N16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4">
         <v>5000</v>
       </c>
-      <c r="D6" s="11">
-        <v>200</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D17" s="4">
+        <v>100</v>
+      </c>
+      <c r="E17" s="3">
+        <v>10</v>
+      </c>
+      <c r="G17" s="8">
+        <v>100</v>
+      </c>
+      <c r="H17" s="8">
         <v>5</v>
       </c>
-      <c r="G6" s="11">
-        <v>5</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1000</v>
-      </c>
-      <c r="I6" s="11">
-        <v>2</v>
-      </c>
-      <c r="J6" s="9">
-        <v>75</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>10</v>
+      <c r="I17" s="8">
+        <v>500</v>
+      </c>
+      <c r="J17" s="8">
+        <v>4</v>
+      </c>
+      <c r="K17" s="9">
+        <v>150</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="13" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3">
-        <v>4</v>
-      </c>
-      <c r="C8" s="11">
-        <v>2500</v>
-      </c>
-      <c r="D8" s="4">
-        <v>100</v>
-      </c>
-      <c r="E8" s="10">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9">
-        <v>200</v>
-      </c>
-      <c r="G8" s="29">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>500</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-      <c r="J8" s="9">
-        <v>200</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L8" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="8">
-        <v>5000</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10">
-        <v>0</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="29">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4">
-        <v>500</v>
-      </c>
-      <c r="I9">
-        <v>4</v>
-      </c>
-      <c r="J9" s="9">
-        <v>250</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="L9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="M35" s="6" t="s">
+      <c r="N35" s="6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="K1:O1"/>
+    <mergeCell ref="E1:K1"/>
+    <mergeCell ref="L1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Created chargeUse variable (default 1), updated stages spreadsheet
</commit_message>
<xml_diff>
--- a/stages.xlsx
+++ b/stages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>playerSpeed</t>
   </si>
@@ -74,12 +74,6 @@
     <t>powerDesc</t>
   </si>
   <si>
-    <t>slowDown</t>
-  </si>
-  <si>
-    <t>playerSpeed = 2</t>
-  </si>
-  <si>
     <t>playerSpeed = 8</t>
   </si>
   <si>
@@ -101,15 +95,6 @@
     <t>increases score multiplier volatility - higher max, lower min, less of in between</t>
   </si>
   <si>
-    <t>Bad idea</t>
-  </si>
-  <si>
-    <t>Diff value from default</t>
-  </si>
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>scoreMult</t>
   </si>
   <si>
@@ -120,9 +105,6 @@
   </si>
   <si>
     <t>stageName</t>
-  </si>
-  <si>
-    <t>Values may req. tweak</t>
   </si>
   <si>
     <r>
@@ -144,9 +126,6 @@
     <t>low healthMax+healthDrain, high healthGain</t>
   </si>
   <si>
-    <t>noShield</t>
-  </si>
-  <si>
     <t>-healthMax</t>
   </si>
   <si>
@@ -250,13 +229,28 @@
   </si>
   <si>
     <t>Charge up shield?</t>
+  </si>
+  <si>
+    <t>5noShield</t>
+  </si>
+  <si>
+    <t>chargeUse</t>
+  </si>
+  <si>
+    <t>1/unit time</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>Stop time, player can still move</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,13 +266,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,22 +274,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -329,27 +306,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -402,82 +364,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
-    <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
-    <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
-    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="5">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
+    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,7 +710,7 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,99 +723,97 @@
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="71.28515625" customWidth="1"/>
-    <col min="14" max="14" width="76.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="5"/>
-    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="71.28515625" customWidth="1"/>
+    <col min="15" max="15" width="76.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="26"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K2" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>28</v>
-      </c>
       <c r="L2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3">
         <v>4</v>
@@ -877,175 +827,184 @@
       <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>10</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>400</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>10</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="4">
         <v>500</v>
       </c>
-      <c r="J3" s="8">
+      <c r="K3" s="7">
         <v>5</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <v>100</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="10">
+        <v>47</v>
+      </c>
+      <c r="B4" s="9">
         <v>6</v>
       </c>
       <c r="C4" s="4">
         <v>5000</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>50</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>20</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="10">
         <v>20</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="10">
         <v>600</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="10">
         <v>5</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10">
         <v>250</v>
       </c>
-      <c r="J4" s="11">
+      <c r="K4" s="10">
         <v>10</v>
       </c>
-      <c r="K4" s="9">
+      <c r="L4" s="8">
         <v>175</v>
       </c>
-      <c r="L4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="N4" s="2" t="s">
+      <c r="M4" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>2500</v>
       </c>
       <c r="D5" s="4">
         <v>100</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>20</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>20</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>800</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="14">
         <v>10</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5">
         <v>500</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5</v>
       </c>
-      <c r="K5" s="9">
+      <c r="L5" s="8">
         <v>200</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>34</v>
+      <c r="M5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>64</v>
-      </c>
       <c r="K6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>23</v>
+        <v>57</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="21">
-        <v>4</v>
+      <c r="A7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="C7" s="4">
         <v>5000</v>
@@ -1062,195 +1021,199 @@
       <c r="G7" s="4">
         <v>400</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>10</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
         <v>500</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="K7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="10">
         <v>150</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>41</v>
+      <c r="M7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="10">
+        <v>1500</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="10">
+        <v>5</v>
+      </c>
+      <c r="J8" s="4">
+        <v>500</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
+      <c r="L8" s="8">
+        <v>250</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>5000</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>200</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>5</v>
       </c>
-      <c r="H11" s="11">
+      <c r="H11" s="10">
         <v>5</v>
       </c>
-      <c r="I11" s="11">
+      <c r="J11" s="10">
         <v>1000</v>
       </c>
-      <c r="J11" s="11">
+      <c r="K11" s="10">
         <v>2</v>
       </c>
-      <c r="K11" s="9">
+      <c r="L11" s="8">
         <v>75</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" t="s">
-        <v>20</v>
-      </c>
-      <c r="N11" s="2" t="s">
+      <c r="M11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N12" s="4"/>
+      <c r="O12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" s="3">
-        <v>4</v>
-      </c>
-      <c r="C12" s="8">
-        <v>5000</v>
-      </c>
-      <c r="D12" s="11">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10">
-        <v>0</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="17">
-        <v>5</v>
-      </c>
-      <c r="I12" s="4">
-        <v>500</v>
-      </c>
-      <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12" s="9">
-        <v>250</v>
-      </c>
-      <c r="L12" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
-      </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4">
+        <v>5000</v>
+      </c>
+      <c r="D13" s="4">
+        <v>100</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10</v>
+      </c>
+      <c r="G13" s="7">
+        <v>100</v>
+      </c>
+      <c r="H13" s="7">
+        <v>5</v>
+      </c>
+      <c r="J13" s="7">
+        <v>500</v>
+      </c>
+      <c r="K13" s="7">
+        <v>4</v>
+      </c>
+      <c r="L13" s="8">
+        <v>150</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" t="s">
         <v>42</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B14" s="3">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4">
-        <v>5000</v>
-      </c>
-      <c r="D14" s="4">
-        <v>100</v>
-      </c>
-      <c r="E14" s="3">
-        <v>10</v>
-      </c>
-      <c r="G14" s="8">
-        <v>100</v>
-      </c>
-      <c r="H14" s="8">
-        <v>5</v>
-      </c>
-      <c r="I14" s="8">
-        <v>500</v>
-      </c>
-      <c r="J14" s="8">
-        <v>4</v>
-      </c>
-      <c r="K14" s="9">
-        <v>150</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" t="s">
-        <v>49</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="O14" s="4" t="s">
-        <v>50</v>
+        <v>2</v>
+      </c>
+      <c r="C14" s="7">
+        <v>10000</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="3">
-        <v>2</v>
-      </c>
-      <c r="C15" s="8">
-        <v>10000</v>
-      </c>
-      <c r="D15" s="8">
-        <v>0</v>
-      </c>
-      <c r="M15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q17" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
-      <c r="N35" s="6" t="s">
+      <c r="O35" s="6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:K1"/>
-    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>